<commit_message>
Fix TNC mode error in SC_summary.py.
</commit_message>
<xml_diff>
--- a/inputs/model/CatVarDict.xlsx
+++ b/inputs/model/CatVarDict.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Clients\BKR\GitRunModel\scripts\summarize\inputs\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\TNC_in_dev\future_improvement\BKR3-19-BB35_NB_2_30%WFH_TNC\inputs\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F26508-3421-4D99-914C-C647B9ED3999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Household" sheetId="1" r:id="rId1"/>
@@ -388,13 +389,13 @@
     <t>Driver+3+Passengers</t>
   </si>
   <si>
-    <t>PRS</t>
+    <t>TNC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,10 +425,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +456,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -474,9 +473,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -514,9 +513,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,7 +550,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -586,7 +585,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,24 +758,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -807,7 +806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -827,7 +826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -847,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9</v>
       </c>
@@ -867,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>5</v>
       </c>
@@ -875,7 +874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>6</v>
       </c>
@@ -883,7 +882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>9</v>
       </c>
@@ -897,30 +896,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -946,7 +945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -980,23 +979,23 @@
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>47</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1030,23 +1029,23 @@
       <c r="K3">
         <v>2</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>48</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>56</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1080,23 +1079,23 @@
       <c r="K4">
         <v>3</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>49</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>57</v>
       </c>
       <c r="O4">
         <v>3</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1112,23 +1111,23 @@
       <c r="K5">
         <v>4</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>50</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" t="s">
         <v>58</v>
       </c>
       <c r="O5">
         <v>8</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1144,17 +1143,17 @@
       <c r="K6">
         <v>5</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>51</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1170,17 +1169,17 @@
       <c r="K7">
         <v>6</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>52</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1196,17 +1195,17 @@
       <c r="K8">
         <v>7</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>53</v>
       </c>
       <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1222,27 +1221,27 @@
       <c r="K9">
         <v>8</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" t="s">
         <v>54</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="K10">
         <v>9</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>39</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1252,24 +1251,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1277,7 +1276,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1285,7 +1284,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1317,7 +1316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1331,23 +1330,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1364,266 +1363,265 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>98</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>98</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>40</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>88</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>99</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>99</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>89</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>100</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>100</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>102</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>103</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>91</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>104</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>92</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>101</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>101</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>105</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>93</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>105</v>
       </c>
       <c r="I8">
         <v>6</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>94</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>106</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>94</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1633,25 +1631,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1674,41 +1672,41 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>98</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>98</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>40</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" t="s">
         <v>107</v>
       </c>
       <c r="M2">
@@ -1718,41 +1716,41 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>88</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>88</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>99</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>99</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" t="s">
         <v>108</v>
       </c>
       <c r="M3">
@@ -1762,41 +1760,41 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>89</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>89</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>100</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>100</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>102</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" t="s">
         <v>109</v>
       </c>
       <c r="M4">
@@ -1806,41 +1804,41 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>90</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>103</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" t="s">
         <v>110</v>
       </c>
       <c r="M5">
@@ -1850,41 +1848,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>91</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>91</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>104</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" t="s">
         <v>111</v>
       </c>
       <c r="M6">
@@ -1894,41 +1892,41 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>92</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>92</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>101</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>101</v>
       </c>
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>105</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" t="s">
         <v>112</v>
       </c>
       <c r="M7">
@@ -1938,29 +1936,29 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>93</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>93</v>
       </c>
       <c r="I8">
         <v>8</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
         <v>106</v>
       </c>
       <c r="K8">
         <v>6</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" t="s">
         <v>113</v>
       </c>
       <c r="M8">
@@ -1970,71 +1968,71 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>94</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>94</v>
       </c>
       <c r="I9">
         <v>9</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
         <v>121</v>
       </c>
       <c r="K9">
         <v>7</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>95</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>96</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>97</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>